<commit_message>
Overwrote the cube to render a pyramid instead, used index buffer in combination with vertex buffer as well.
</commit_message>
<xml_diff>
--- a/Brennan Rodriguez Dev IV Project Rubric.xlsx
+++ b/Brennan Rodriguez Dev IV Project Rubric.xlsx
@@ -933,7 +933,7 @@
   <dimension ref="A1:L110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3019,7 +3019,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Procedural model rendering implemented (first thing in the excel)
</commit_message>
<xml_diff>
--- a/Brennan Rodriguez Dev IV Project Rubric.xlsx
+++ b/Brennan Rodriguez Dev IV Project Rubric.xlsx
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="96">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -366,6 +366,12 @@
   </si>
   <si>
     <t>Student Git Address: https://github.com/Kertic/Graphics2Project.git</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -933,7 +939,7 @@
   <dimension ref="A1:L110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,15 +1053,19 @@
       <c r="D4" s="5">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3"/>
+      <c r="E4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="G4" s="16">
         <f t="shared" ref="G4:G30" si="0" xml:space="preserve"> IF(EXACT(F4,"X"),IF(EXACT(E4,"I"),$B4,IF(EXACT(E4,"II"),$C4,IF(EXACT(E4,"III"),$D4,0))),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E81,"=I",G4:G81) + SUMIF(C83:C84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=I",G4:G81) + SUMIF(C83:C84, "X",B83:B84))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E81,"=II",G4:G81) + SUMIF(D83:D84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=II",G4:G81) + SUMIF(D83:D84, "X",B83:B84))</f>
@@ -1071,7 +1081,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G81) + SUMIF(C83:C84, "X",B83:B84) + SUMIF(D83:D84, "X",B83:B84) + SUMIF(E83:E84, "X",B83:B84)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1196,7 +1206,7 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 18, IF(K4+H4 &gt; 18, 18- H4, K4),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
@@ -3019,7 +3029,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Added custom vertex shader to transform models independently. Added instanced drawing for the procedural pyramid.
</commit_message>
<xml_diff>
--- a/Brennan Rodriguez Dev IV Project Rubric.xlsx
+++ b/Brennan Rodriguez Dev IV Project Rubric.xlsx
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="98">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -372,6 +372,12 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>https://www.opengl.org/discussion_boards/showthread.php/198728-loading-obj-file-how-to-triangularize-polygons - Dealing with non-triangulated OBJs</t>
+  </si>
+  <si>
+    <t>https://www.braynzarsoft.net/viewtutorial/q16390-33-instancing-with-indexed-primitives - Instanced Primitives</t>
   </si>
 </sst>
 </file>
@@ -938,8 +944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,7 +1071,7 @@
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E81,"=I",G4:G81) + SUMIF(C83:C84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=I",G4:G81) + SUMIF(C83:C84, "X",B83:B84))</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E81,"=II",G4:G81) + SUMIF(D83:D84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=II",G4:G81) + SUMIF(D83:D84, "X",B83:B84))</f>
@@ -1081,7 +1087,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G81) + SUMIF(C83:C84, "X",B83:B84) + SUMIF(D83:D84, "X",B83:B84) + SUMIF(E83:E84, "X",B83:B84)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1097,11 +1103,15 @@
       <c r="D5" s="5">
         <v>2</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="G5" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>27</v>
@@ -1206,7 +1216,7 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 18, IF(K4+H4 &gt; 18, 18- H4, K4),0)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
@@ -2939,10 +2949,14 @@
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A88" s="12"/>
+      <c r="A88" s="12" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A89" s="12"/>
+      <c r="A89" s="12" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="12"/>

</xml_diff>

<commit_message>
Filled out rubric for milestone 1
</commit_message>
<xml_diff>
--- a/Brennan Rodriguez Dev IV Project Rubric.xlsx
+++ b/Brennan Rodriguez Dev IV Project Rubric.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-465" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="-465" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="98">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -377,7 +377,7 @@
     <t>https://www.opengl.org/discussion_boards/showthread.php/198728-loading-obj-file-how-to-triangularize-polygons - Dealing with non-triangulated OBJs</t>
   </si>
   <si>
-    <t>https://www.braynzarsoft.net/viewtutorial/q16390-33-instancing-with-indexed-primitives - Instanced Primitives</t>
+    <t>https://www.braynzarsoft.net/viewtutorial/q16390-33-instancing-with-indexed-primitives - Instanced Drawing of shapes</t>
   </si>
 </sst>
 </file>
@@ -944,8 +944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="A92" sqref="A92"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,7 +1071,7 @@
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E81,"=I",G4:G81) + SUMIF(C83:C84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=I",G4:G81) + SUMIF(C83:C84, "X",B83:B84))</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E81,"=II",G4:G81) + SUMIF(D83:D84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=II",G4:G81) + SUMIF(D83:D84, "X",B83:B84))</f>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G81) + SUMIF(C83:C84, "X",B83:B84) + SUMIF(D83:D84, "X",B83:B84) + SUMIF(E83:E84, "X",B83:B84)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1140,11 +1140,15 @@
       <c r="D6" s="5">
         <v>3</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="G6" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E81,"=I",G4:G81) + SUMIF(C83:C84, "X",B83:B84)  &gt; 18, SUMIF(E4:E81,"=I",G4:G81) + SUMIF(C83:C84, "X",B83:B84) - 18,0)</f>
@@ -1216,7 +1220,7 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 18, IF(K4+H4 &gt; 18, 18- H4, K4),0)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
@@ -2886,7 +2890,9 @@
       <c r="B83" s="6">
         <v>2</v>
       </c>
-      <c r="C83" s="3"/>
+      <c r="C83" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
       <c r="F83" s="5"/>
@@ -2904,7 +2910,9 @@
       <c r="B84" s="6">
         <v>1</v>
       </c>
-      <c r="C84" s="3"/>
+      <c r="C84" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
       <c r="F84" s="5"/>

</xml_diff>

<commit_message>
Added dynamic light support
</commit_message>
<xml_diff>
--- a/Brennan Rodriguez Dev IV Project Rubric.xlsx
+++ b/Brennan Rodriguez Dev IV Project Rubric.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="-465" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-465" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="99">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -378,6 +378,9 @@
   </si>
   <si>
     <t>https://www.braynzarsoft.net/viewtutorial/q16390-33-instancing-with-indexed-primitives - Instanced Drawing of shapes</t>
+  </si>
+  <si>
+    <t>II</t>
   </si>
 </sst>
 </file>
@@ -944,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,7 +1078,7 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E81,"=II",G4:G81) + SUMIF(D83:D84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=II",G4:G81) + SUMIF(D83:D84, "X",B83:B84))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84))</f>
@@ -1087,7 +1090,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G81) + SUMIF(C83:C84, "X",B83:B84) + SUMIF(D83:D84, "X",B83:B84) + SUMIF(E83:E84, "X",B83:B84)</f>
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1224,7 +1227,7 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
@@ -1611,11 +1614,15 @@
       <c r="D25" s="5">
         <v>2</v>
       </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="3"/>
+      <c r="E25" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="G25" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
@@ -1636,11 +1643,15 @@
       <c r="D26" s="5">
         <v>2</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="3"/>
+      <c r="E26" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="G26" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
@@ -1661,11 +1672,15 @@
       <c r="D27" s="5">
         <v>2</v>
       </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="3"/>
+      <c r="E27" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="G27" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
@@ -1711,11 +1726,15 @@
       <c r="D29" s="5">
         <v>1</v>
       </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="3"/>
+      <c r="E29" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="G29" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
@@ -1736,11 +1755,15 @@
       <c r="D30" s="5">
         <v>1</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="3"/>
+      <c r="E30" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="G30" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
@@ -1761,11 +1784,15 @@
       <c r="D31" s="5">
         <v>1</v>
       </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="3"/>
+      <c r="E31" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="G31" s="16">
         <f t="shared" ref="G31:G65" si="1" xml:space="preserve"> IF(EXACT(F31,"X"),IF(EXACT(E31,"I"),$B31,IF(EXACT(E31,"II"),$C31,IF(EXACT(E31,"III"),$D31,0))),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -3051,7 +3078,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Changed loaded model to be more complex than pyramid
</commit_message>
<xml_diff>
--- a/Brennan Rodriguez Dev IV Project Rubric.xlsx
+++ b/Brennan Rodriguez Dev IV Project Rubric.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-465" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="101">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -381,6 +381,12 @@
   </si>
   <si>
     <t>II</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/windows/uwp/gaming/applying-textures-to-primitives - Setting up sampler discription</t>
+  </si>
+  <si>
+    <t>III</t>
   </si>
 </sst>
 </file>
@@ -947,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,7 +1088,7 @@
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
@@ -1090,7 +1096,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G81) + SUMIF(C83:C84, "X",B83:B84) + SUMIF(D83:D84, "X",B83:B84) + SUMIF(E83:E84, "X",B83:B84)</f>
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1231,7 +1237,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1436,11 +1442,15 @@
       <c r="D17" s="5">
         <v>2</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="3"/>
+      <c r="E17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="G17" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
@@ -2927,7 +2937,9 @@
       <c r="D83" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E83" s="3"/>
+      <c r="E83" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="F83" s="5"/>
       <c r="G83" s="5"/>
       <c r="H83" s="5"/>
@@ -2949,7 +2961,9 @@
       <c r="D84" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E84" s="3"/>
+      <c r="E84" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="F84" s="5"/>
       <c r="G84" s="5"/>
       <c r="H84" s="5"/>
@@ -3002,7 +3016,9 @@
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A90" s="12"/>
+      <c r="A90" s="12" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="12"/>
@@ -3086,7 +3102,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Got dynamic detail working, just need to implement height map behavior
</commit_message>
<xml_diff>
--- a/Brennan Rodriguez Dev IV Project Rubric.xlsx
+++ b/Brennan Rodriguez Dev IV Project Rubric.xlsx
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="102">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -387,6 +387,9 @@
   </si>
   <si>
     <t>III</t>
+  </si>
+  <si>
+    <t>http://richardssoftware.net/Home/Post/19 - Billboarding algorithm</t>
   </si>
 </sst>
 </file>
@@ -953,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,7 +1091,7 @@
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84))</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
@@ -1096,7 +1099,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G81) + SUMIF(C83:C84, "X",B83:B84) + SUMIF(D83:D84, "X",B83:B84) + SUMIF(E83:E84, "X",B83:B84)</f>
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1190,11 +1193,15 @@
       <c r="D7" s="5">
         <v>3</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
+      <c r="E7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="G7" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>23</v>
@@ -1237,7 +1244,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -3021,7 +3028,9 @@
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A91" s="12"/>
+      <c r="A91" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="12"/>
@@ -3102,7 +3111,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Fixed billboarding and animated clouds
</commit_message>
<xml_diff>
--- a/Brennan Rodriguez Dev IV Project Rubric.xlsx
+++ b/Brennan Rodriguez Dev IV Project Rubric.xlsx
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="103">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -959,8 +959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A93" sqref="A93"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,11 +1098,11 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G81) + SUMIF(C83:C84, "X",B83:B84) + SUMIF(D83:D84, "X",B83:B84) + SUMIF(E83:E84, "X",B83:B84)</f>
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1175,7 +1175,7 @@
       </c>
       <c r="J6" s="17">
         <f>IF(SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84) &gt; 18, SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84) - 18,0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="15">
@@ -1243,11 +1243,11 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 18, IF(K4+H4 &gt; 18, 18- H4, K4),0)</f>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
@@ -1269,11 +1269,15 @@
       <c r="D9" s="5">
         <v>1</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
+      <c r="E9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="G9" s="16">
         <f xml:space="preserve"> IF(EXACT(F9,"X"),IF(EXACT(E9,"I"),$B9,IF(EXACT(E9,"II"),$C9,IF(EXACT(E9,"III"),$D9,0))),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="19" t="s">
         <v>26</v>
@@ -1308,7 +1312,7 @@
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 18 &gt; 0, K4+H4 - 18, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 18 &gt; 0, H10+I4 - 18, 0)</f>
@@ -1535,11 +1539,15 @@
       <c r="D20" s="5">
         <v>3</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="3"/>
+      <c r="E20" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="G20" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -3124,7 +3132,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Added multi-texturing based on multiply and added transparent masking
</commit_message>
<xml_diff>
--- a/Brennan Rodriguez Dev IV Project Rubric.xlsx
+++ b/Brennan Rodriguez Dev IV Project Rubric.xlsx
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="103">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -959,8 +959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,11 +1098,11 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G81) + SUMIF(C83:C84, "X",B83:B84) + SUMIF(D83:D84, "X",B83:B84) + SUMIF(E83:E84, "X",B83:B84)</f>
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1175,12 +1175,12 @@
       </c>
       <c r="J6" s="17">
         <f>IF(SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84) &gt; 18, SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84) - 18,0)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="15">
         <f>IF(L4 &gt; 54, SUM(-54,L4),0)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1312,15 +1312,15 @@
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 18 &gt; 0, K4+H4 - 18, 0)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 18 &gt; 0, H10+I4 - 18, 0)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J10" s="19">
         <f>IF(I10+J4 - 18 &gt; 0, I10+J4 - 18, 0)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1489,11 +1489,15 @@
       <c r="D18" s="5">
         <v>2</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="3"/>
+      <c r="E18" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="G18" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -1568,11 +1572,15 @@
       <c r="D21" s="5">
         <v>4</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="3"/>
+      <c r="E21" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="G21" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>

</xml_diff>